<commit_message>
add in changes from shiny merge app branch and refactor
</commit_message>
<xml_diff>
--- a/variable_names_new/column_names.xlsx
+++ b/variable_names_new/column_names.xlsx
@@ -372,2800 +372,4515 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>council</t>
+          <t>_010000</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Year</t>
+          <t>_015</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0-15</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CLIMATE1</t>
+          <t>_015000</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Up to £15,000</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>_1639</t>
+          <t>_06000</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Up to £6,000</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>_4064</t>
+          <t>_1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>_65</t>
+          <t>_1000115000</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>£10,001 to £15,000</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>_All</t>
+          <t>_1000120000</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>£10,001 to £20,000</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>_11to20years</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11 to 20 years</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>_2013</t>
+          <t>_120mostdeprived</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1 - 20% most deprived</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>_2014</t>
+          <t>_120MostDeprived</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1 - 20% most deprived</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>_2015</t>
+          <t>_13years</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>13 years</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>_2016</t>
+          <t>_1500120000</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1500120000</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>_2017</t>
+          <t>_1500130000</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1500130000</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>_2018</t>
+          <t>_1624</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>16 to 24</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>greenfar13</t>
+          <t>_1639</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16 to 39</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>_NAME_</t>
+          <t>_16to39</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16 to 39</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>_2009_2010</t>
+          <t>_1999</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>1999</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>_2011</t>
+          <t>_19992000</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>1999/2000</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>_2012</t>
+          <t>_1MostDeprived</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>1 - 20% most deprived</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>voluntee</t>
+          <t>_1to2years</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>1 to 2 years</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>_1MostDeprived</t>
+          <t>_2</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>_2</t>
+          <t>_2000</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2000</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>_3</t>
+          <t>_2000125000</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>£20,001 to £25,000</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>_4</t>
+          <t>_2000130000</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>£20,001 to £30,000</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>_5LeastDeprived</t>
+          <t>_2001</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2001</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>_20012002</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2001/2002</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>volinform</t>
+          <t>_2002</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2002</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>_Male</t>
+          <t>_2003</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2003</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>_Female</t>
+          <t>_20032004</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2003/2004</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>_Inanotherway</t>
+          <t>_2004</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2004</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>_Refused</t>
+          <t>_2005</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2005</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>_Base</t>
+          <t>_20052006</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2005/2006</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CultAny</t>
+          <t>_2006</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2006</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>_010000</t>
+          <t>_2007</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2007</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>_1000120000</t>
+          <t>_20072008</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2007/2008</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>_2000130000</t>
+          <t>_2008</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2008</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>_Over30000</t>
+          <t>_2009</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2009</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>_Yesalot</t>
+          <t>_2009_2010</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2009/2010</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>_Yesalittle</t>
+          <t>_20092010</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2009/2010</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>_Yesbutnoreducedcapacity</t>
+          <t>_2010</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2010</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>_None</t>
+          <t>_2011</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2011</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>_AllAdults</t>
+          <t>_2012</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2012</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>_HNCHNDorDegreeProf.Qual</t>
+          <t>_2013</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2013</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>_O_StandHigherAlevelorequivalent</t>
+          <t>_2014</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2014</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>_Otherqualification</t>
+          <t>_2015</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2015</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>_Noqualifications</t>
+          <t>_2016</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2016</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>_Qualificationsnotknown</t>
+          <t>_2017</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2017</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>_120MostDeprived</t>
+          <t>_2018</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2018</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>_520LeastDeprived</t>
+          <t>_20leastdeprived</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>20% least deprived</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>ha5</t>
+          <t>_20mostdeprived</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>20% most deprived</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>_19992000</t>
+          <t>_2500130000</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>£25,001 to £30,000</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>_20012002</t>
+          <t>_2534</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>25-34</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>_20032004</t>
+          <t>_3</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>_20052006</t>
+          <t>_3000135000</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>£30,001 to £35,000</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>_20072008</t>
+          <t>_3000140000</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>£30,001 to £40,000</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>_20092010</t>
+          <t>_3500140000</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>£35,001 to £40,000</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>_3544</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>35 to 44</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>ha7</t>
+          <t>_35years</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>35 years</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>rndrel09</t>
+          <t>_3to4years</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>3 to 4 years</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>tenure</t>
+          <t>_4</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>_1999</t>
+          <t>_4000150000</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>£40,001 to £50,000</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>_2000</t>
+          <t>_4059</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>40 to 59</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>_2001</t>
+          <t>_4064</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>40 to 64</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>_2002</t>
+          <t>_40to59</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>40 to 59</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>_2003</t>
+          <t>_4559</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>45 to 59</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>_2004</t>
+          <t>_5000160000</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>£50,001 to £60,000</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>_2005</t>
+          <t>_520leastdeprived</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>5 - 20% least deprived</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>_2006</t>
+          <t>_520LeastDeprived</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>5 - 20% least deprived</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>_2007</t>
+          <t>_5LeastDeprived</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>5 - 20% least deprived</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>_2008</t>
+          <t>_5to10years</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>5 to 10 years</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>_2009</t>
+          <t>_60</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>60 plus</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>_2010</t>
+          <t>_6000170000</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>£60,001 to £70,000</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>hihage</t>
+          <t>_600110000</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>£6,001 to £10,000</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>pa1</t>
+          <t>_6074</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>60 to 74</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>rb1</t>
+          <t>_610years</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>_20mostdeprived</t>
+          <t>_65</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>65 plus</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>_20leastdeprived</t>
+          <t>_7000180000</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>£70,001 to £80,000</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>LABEL</t>
+          <t>_75</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>75 plus</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Perception</t>
+          <t>_a.0cars</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>0 cars</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Experience</t>
+          <t>_a.1624</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>16-24</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>_ManBoy</t>
+          <t>_a.1bedroom</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>1 bedroom</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>_WomanGirl</t>
+          <t>_a.1person</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>1 person</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>_Inanotherway(ifyouwouldliketopl</t>
+          <t>_a.house</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>House</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>_Refused(spontaneous)</t>
+          <t>_a.OwnerOccupier</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Owner occupier</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>working_adults</t>
+          <t>_a.WhiteScottish</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>White Scottish</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>_Yeshavechildren</t>
+          <t>_Accessiblerural</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Accessible rural</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>_Nochildren</t>
+          <t>_Accessiblesmalltowns</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Accessible small towns</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>hk2</t>
+          <t>_All</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>_Upto15000</t>
+          <t>_All_1</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>_1500130000</t>
+          <t>_All_2</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>_SingleadultSmalladultLargeadult</t>
+          <t>_All_Age</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>_SingleparentSmallfamilyLargefam</t>
+          <t>_All_Gender</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>_OldersmallerSingleolder</t>
+          <t>_AllAdults</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>_Manageswell</t>
+          <t>_AllAge</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>_Getsby</t>
+          <t>_AllGender</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>_Doesnotmanagewell</t>
+          <t>_AllOwner</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>hc6</t>
+          <t>_AllSIMD</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>net1</t>
+          <t>_AllSocial</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>AnySport</t>
+          <t>_Anequalmixofincomesources</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>An equal mix of income sources</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>AnySportExclWalking</t>
+          <t>_Anotherway</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Another way</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Walking</t>
+          <t>_Atleastonceaweek</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>At least once a week</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>BaseMin</t>
+          <t>_Atschool</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>At school</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>SPRT3B</t>
+          <t>_b.1car</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>1 car</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>outdoor</t>
+          <t>_b.2534</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>25-34</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>_VeryBadBad</t>
+          <t>_b.2bedrooms</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>2 bedrooms</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>_VeryGoodGood</t>
+          <t>_b.2people</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>2 people</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>_Fair</t>
+          <t>_b.flat</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Flat</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>_120mostdeprived</t>
+          <t>_b.Ownedoutright</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Owned outright</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>_520leastdeprived</t>
+          <t>_b.Privaterent</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Private rent</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>RESPONSE</t>
+          <t>_b.WhiteotherBritish</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>White/Other British</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>_UrbanAreas</t>
+          <t>_Base</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Base</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>_RuralAreas</t>
+          <t>_Buyingwithhelpofloanmortgage</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Buying with help of loan/mortgage</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>CLIMATE2_A</t>
+          <t>_c.2cars</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>2 cars</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>CLIMATE2_B</t>
+          <t>_c.3544</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>35-44</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>CLIMATE2_C</t>
+          <t>_c.3bedrooms</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>3 bedrooms</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>CLIMATE2_D</t>
+          <t>_c.3people</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>3 people</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>vol42018</t>
+          <t>_c.Buyingwithhelpofloanmortgage</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Buying with help of loan/mortgage</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>_Selfemployedfullparttimeemploym</t>
+          <t>_c.other</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>_Other</t>
+          <t>_c.SocialSector</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Social sector</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>_Permanentlyretiredfromwork</t>
+          <t>_c.WhitePolish</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>White/Polish</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>_Largeurbanareas</t>
+          <t>_CantaffordcurrenthousingWouldli</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>_Otherurbanareas</t>
+          <t>_d.4559</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>45-59</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>_Accessiblesmalltowns</t>
+          <t>_d.4bedrooms</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>4 bedrooms</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>_Remotesmalltowns</t>
+          <t>_d.4people</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>4 people</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>_Accessiblerural</t>
+          <t>_d.Other</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>_Remoterural</t>
+          <t>_d.PrivateRented</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Private rented</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>voliv2</t>
+          <t>_d.Whiteother</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>White/Other</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>voliv3</t>
+          <t>_DegreeProfessionalQualification</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Degree / professional qualification</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>vol32018</t>
+          <t>_Doesnotmanagewell</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Does not manage well</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>_4059</t>
+          <t>_Dontknow</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Don't know</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>_60</t>
+          <t>_DontKnow</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Don't know</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>var</t>
+          <t>_Dontknowrefused</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Don't Know/Refused</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>_Atleastonceaweek</t>
+          <t>_e.6074</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>60-74</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>_onceaweekbutatleastonceamonth</t>
+          <t>_e.AnyMixedorMultipleEthnicGroup</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Any mixed or multiple ethnic group</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>_onceamonthandwithinyear</t>
+          <t>_e.PrivateRent</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Private rent</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>_Dontknow</t>
+          <t>_e.Rent–LA</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Rent Local Authority</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>base</t>
+          <t>_Employedfulltime</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Employed full time</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>response</t>
+          <t>_Employedparttime</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Employed part time</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>randstat</t>
+          <t>_f.AsianAsianScottishorAsianBrit</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Asian/Asian Scottish/Asian British</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>_015</t>
+          <t>_f.RentHACoop</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Rent Housing Association/Co-op</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>_1624</t>
+          <t>_Fair</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Fair</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>_2534</t>
+          <t>_Fairlydissatisfied</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Fairly dissatisfied</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>_3544</t>
+          <t>_Fairlygood</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Fairly good</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>_4559</t>
+          <t>_Fairlypoor</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Faily poor</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>_6074</t>
+          <t>_Fairlysatisfied</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Faily satisfied</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>_75</t>
+          <t>_Fairlystrongly</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Fairly strongly</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>hhtype</t>
+          <t>_Female</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Female</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>hb1</t>
+          <t>_g.75</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>75+</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>SIMDquintiles</t>
+          <t>_g.AfricanCaribbeanorBlack</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Afican Caribbean or Black</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>shs_6cla</t>
+          <t>_g.Localauthority</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Local Authority</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>tothinc</t>
+          <t>_g.Other</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>ha6</t>
+          <t>_Getsby</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Gets by</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>hf1an</t>
+          <t>_Governmentworkortrainingscheme</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Government work or training scheme</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>rg5a</t>
+          <t>_h.HousingassociationCoopCharita</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Housing association/Co-op/Charitable trust</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>randeth</t>
+          <t>_h.Inparentalfamilyhome</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>In parental family home</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Alladults</t>
+          <t>_h.OtherEthnicGroup</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Other ethnic group</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Workingageadults</t>
+          <t>_HigherAlevelOGradeStandardGrade</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Higher/A level/O Grade/Standard Grade</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>rand_id</t>
+          <t>_HNCHNDorDegreeProf.Qual</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>HNC/HND/Degree/ Prof.Qualification</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>tenurealt</t>
+          <t>_Housingassociation</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Housing association</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>_Ownedoutright</t>
+          <t>_HousingAssociationRent</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Housing Association Rent</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>_Buyingwithhelpofloanmortgage</t>
+          <t>_i.Dontknow</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Don't Know</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>_AllOwner</t>
+          <t>_i.Other</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>_PrivateRent</t>
+          <t>_Identifiedinanotherway</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Identified in another way</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>_Localauthority</t>
+          <t>_Inanotherway</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>In another way</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>_Housingassociation</t>
+          <t>_Inanotherway(ifyouwouldliketopl</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>In another way</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>_AllSocial</t>
+          <t>_Infurtherhighereducation</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>In further higher education</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>_Yesonahousinglist</t>
+          <t>_j.Refused</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Refused</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>_Dontknowrefused</t>
+          <t>_landlord</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Landlord</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>_Nonotonahousinglist</t>
+          <t>_Largeadult</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Large adult</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>_DontKnow</t>
+          <t>_Largefamily</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Large family</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>_Yes</t>
+          <t>_Larger</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Larger</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>_No</t>
+          <t>_Largeurbanareas</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Large urban areas</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>_1</t>
+          <t>_Lessthanayear</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Less than a year</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>_Lessthanayear</t>
+          <t>_Lessthanoneyear</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Less than one year</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>_13years</t>
+          <t>_Lettingagent</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Letting agent</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>_35years</t>
+          <t>_Localauthority</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Local Authority</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>_610years</t>
+          <t>_LocalAuthorityRent</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Local Authority rent</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>_Morethan10years</t>
+          <t>_Longtermcondition_1</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Yes long-term condition</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>_Threatenedwithhomelessness</t>
+          <t>_Longtermcondition_2</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Yes ('excluding permanently sick or disabled')</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>_Tomovetomyownpropertyawayfrompa</t>
+          <t>_Lookingafterthehomeorfamily</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Looking after the home/family</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>_CantaffordcurrenthousingWouldli</t>
+          <t>_Mainincomefrombenefits</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Main income from benefits</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>_TomovetoadifferentareaAntisocia</t>
+          <t>_Mainincomefromearnings</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Main income from earnings</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>_TomovetoadifferentareaTobeneare</t>
+          <t>_Mainincomefromothersources</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Main income from other sources</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>_TomovetoadifferentareaToabetter</t>
+          <t>_Male</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Male</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>_TomovetoadifferentareaForworkop</t>
+          <t>_Manageswell</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Manages well</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>_TomovetoadifferentareaSchoolcat</t>
+          <t>_ManBoy</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Man / Boy</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>_TomovetoadifferentareaOtherreas</t>
+          <t>_Morethan10years</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>More than 10 years</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>_TomovetoadifferentpropertyBigge</t>
+          <t>_Morethan20years</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>More than 20 years</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>_TomovetoadifferentpropertyNeeda</t>
+          <t>_NAME_</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>_TomovetoadifferentpropertyNeedg</t>
+          <t>_Neitheragreenordisagree</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Neither agree nor disagree</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>_TomovetoadifferentpropertyOther</t>
+          <t>_Neithersatisfiednordissatisfied</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Neither satisfied nor dissatisfied</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>_OtherOther(specify)</t>
+          <t>_No</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>_OtherDontknow</t>
+          <t>_No–dontexpecttomove</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>No - don't expect to move</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>_OtherRefused</t>
+          <t>_No_Disc</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>No Discrimination</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>ra15</t>
+          <t>_No_Discrim</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>No Discrimination</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>hhtype_new</t>
+          <t>_No_Harass</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>No Harassment</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>ra1</t>
+          <t>_Nochildren</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>No children</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>_urban</t>
+          <t>_nolongtermcondition_1</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>No long-term condition</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>_smalltown</t>
+          <t>_nolongtermcondition_2</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>No ('excluding permanently sick or disabled')</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>_rural</t>
+          <t>_None</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>previoustenure</t>
+          <t>_Nonotonahousinglist</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>No not on a housing list</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Council</t>
+          <t>_Noopinion</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>No opinion</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Category</t>
+          <t>_Noqualifications</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>No qualifications</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>1999</t>
+          <t>_Notatallstrongly</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Not at all strongly</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>_Notverystrongly</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Not very strongly</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>2001</t>
+          <t>_O_StandHigherAlevelorequivalent</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>O grade/Standard grade/Higher/A level/Equivalent</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>2002</t>
+          <t>_Oldersmaller</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Older smaller</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>2003</t>
+          <t>_OldersmallerSingleolder</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Older smaller / Single older</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>2004</t>
+          <t>_onceamonthandwithinyear</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Once a month and within year</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>_onceaweekbutatleastonceamonth</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Once a week but at least once a month</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>2006</t>
+          <t>_Other</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>2007</t>
+          <t>_OtherDontknow</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Other/Don't Know</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>2008</t>
+          <t>_OtherOther(specify)</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Other (please specify)</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>2009</t>
+          <t>_Otherpleasesaywhat(specify)</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Other (please specify)</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>_Otherqualification</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Other qualification</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>2011</t>
+          <t>_OtherRefused</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Other/Refused</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>_Otherurbanareas</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Other urban areas</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>2013</t>
+          <t>_Over30000</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Over £30,000</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>_Over40000</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Over £40,000</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>_Over80000</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Over £80,000</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>_Ownbuyownhome</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Own / buy own home</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>_Owned</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Owned</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>_Ownedoutright</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Owned outright</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>_a.house</t>
+          <t>_Owneroccupied</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Owner occupied</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>_b.flat</t>
+          <t>_OwnerOccupier</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Owner occupier</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>_c.other</t>
+          <t>_Permanentlyretiredfromwork</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Permanently retired from work</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>_a.1bedroom</t>
+          <t>_Permanentlysickordisabled</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Permanently sick or disabled</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>_b.2bedrooms</t>
+          <t>_PreschoolNotyetatschool</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Preschool/Not yet at school</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>_c.3bedrooms</t>
+          <t>_PrivateRent</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Private rent</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>_d.4bedrooms</t>
+          <t>_Privaterented</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Private rented</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>_a.1person</t>
+          <t>_PrivateRented</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Private rented</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>_b.2people</t>
+          <t>_Qualificationsnotknown</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Qualifications not known</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>_c.3people</t>
+          <t>_Refusal</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Refusal</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>_d.4people</t>
+          <t>_Refused</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Refused</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>_Singleadult</t>
+          <t>_Refused(spontaneous)</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>Refused</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>_Smalladult</t>
+          <t>_RefusedDontknow</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Refused/Don't Know</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>_Singleparent</t>
+          <t>_Remoterural</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>Remote rural</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>_Smallfamily</t>
+          <t>_Remotesmalltowns</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>Remote small towns</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>_Largefamily</t>
+          <t>_Rentprivatelandlord</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Rent - private landlord</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>_Largeadult</t>
+          <t>_Rentsocialhousing</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Rent - social housing</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>_Oldersmaller</t>
+          <t>_rural</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>_Singlepensioner</t>
+          <t>_Ruralareas</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Rural areas</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>_a.1624</t>
+          <t>_RuralAreas</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>Rural areas</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>_b.2534</t>
+          <t>_Samesizeascurrent</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>Same size as current</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>_c.3544</t>
+          <t>_Selfemployed</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Self employed</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>_d.4559</t>
+          <t>_Selfemployedfullparttimeemploym</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>Self employed/full-/part-/time employment</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>_e.6074</t>
+          <t>_ShelteredSupported</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>Sheltered Supported</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>_g.75</t>
+          <t>_Singleadult</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>Single adult</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>_a.0cars</t>
+          <t>_SingleadultSmalladultLargeadult</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Single adult / small adult small / Large adult</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>_b.1car</t>
+          <t>_Singleparent</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Single parent</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>_c.2cars</t>
+          <t>_SingleparentSmallfamilyLargefam</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>Single parent / small family / large family</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>_06000</t>
+          <t>_Singlepensioner</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>Single pensioner</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>_600110000</t>
+          <t>_Smalladult</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>Small adult</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>_1000115000</t>
+          <t>_Smaller</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>Smaller</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>_1500120000</t>
+          <t>_Smallfamily</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>Small family</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>_2000125000</t>
+          <t>_smalltown</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>Small town</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>_2500130000</t>
+          <t>_Socialrented</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>Social rented</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>_3000135000</t>
+          <t>_SocialRented</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>Social rented</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>_3500140000</t>
+          <t>_Stronglyagree</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>Strongly agree</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>_4000150000</t>
+          <t>_Stronglydisagree</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>Strongly disagree</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>_5000160000</t>
+          <t>_Tendtoagree</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>Tend to agree</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>_6000170000</t>
+          <t>_Tendtodisagree</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>Tend to disagree</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>_7000180000</t>
+          <t>_Threatenedwithhomelessness</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>Threatened with homelessness</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>_Over80000</t>
+          <t>_Tojoinanexistingfamilyorhouseho</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>To join an existing family or household</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>_RefusedDontknow</t>
+          <t>_TomovetoadifferentareaAntisocia</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>_a.WhiteScottish</t>
+          <t>_TomovetoadifferentareaForworkop</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>_b.WhiteotherBritish</t>
+          <t>_TomovetoadifferentareaOtherreas</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>_c.WhitePolish</t>
+          <t>_TomovetoadifferentareaSchoolcat</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>_d.Whiteother</t>
+          <t>_TomovetoadifferentareaToabetter</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>_e.AnyMixedorMultipleEthnicGroup</t>
+          <t>_TomovetoadifferentareaTobeneare</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>_f.AsianAsianScottishorAsianBrit</t>
+          <t>_TomovetoadifferentpropertyBigge</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>_g.AfricanCaribbeanorBlack</t>
+          <t>_TomovetoadifferentpropertyNeeda</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>_h.OtherEthnicGroup</t>
+          <t>_TomovetoadifferentpropertyNeedg</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>_i.Dontknow</t>
+          <t>_TomovetoadifferentpropertyOther</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>_j.Refused</t>
+          <t>_Tomovetomyownpropertyawayfrompa</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>_Selfemployed</t>
+          <t>_Tooccupytheentireproperty</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>To occupy the entire property</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>_Employedfulltime</t>
+          <t>_Unabletoworkbecauseofshorttermi</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Unable to work because short term illness</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>_Employedparttime</t>
+          <t>_Unemployedandseekingwork</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>Unemployed and seeking work</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>_Lookingafterthehomeorfamily</t>
+          <t>_Upto15000</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>Up to £15,000</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>_Unemployedandseekingwork</t>
+          <t>_urban</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>Urban</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>_Atschool</t>
+          <t>_Urbanareas</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>Urban areas</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>_Infurtherhighereducation</t>
+          <t>_UrbanAreas</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>Urban areas</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>_Governmentworkortrainingscheme</t>
+          <t>_VeryBadBad</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>Bad / very bad</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>_Permanentlysickordisabled</t>
+          <t>_Verydissatisfied</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>Very dissatisfied</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>_Unabletoworkbecauseofshorttermi</t>
+          <t>_Verygood</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>Very good</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>_PreschoolNotyetatschool</t>
+          <t>_VeryGoodGood</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>Good / very good</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>_Otherpleasesaywhat(specify)</t>
+          <t>_Verypoor</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>Very poor</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>_Lessthanoneyear</t>
+          <t>_Verysatisfied</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>Very satisfied</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>_1to2years</t>
+          <t>_Verystrongly</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>Very strongly</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>_3to4years</t>
+          <t>_WomanGirl</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>Woman / Girl</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>_5to10years</t>
+          <t>_Yes</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>_11to20years</t>
+          <t>_Yes–inthenextsixmonths</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>Yes  in the next six months</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>_Morethan20years</t>
+          <t>_Yes–morethan5years</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>Yes more than 5 years</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>_b.Ownedoutright</t>
+          <t>_Yes–over1yearlessthan2years</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>Yes over 1 year,  less than 2 years</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>_c.Buyingwithhelpofloanmortgage</t>
+          <t>_Yes–over2yearslessthan3years</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>Yes over 2 years, less than 3 years</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>_g.Localauthority</t>
+          <t>_Yes–over3yearslessthan4years</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>Yes over 3 years, less than 4 years</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>_h.HousingassociationCoopCharita</t>
+          <t>_Yes–over4yearslessthan5years</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>Yes over 4 years, less than 5 years</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>_e.PrivateRent</t>
+          <t>_Yes–over6monthstolessthan1year</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>Yes over 6 months, less than 1 year</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>_i.Other</t>
+          <t>_Yes_Disc</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>Yes Discrimination</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>_a.OwnerOccupier</t>
+          <t>_Yes_Discrim</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>Yes Discrimination</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>_c.SocialSector</t>
+          <t>_Yes_Harass</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Yes Harassment</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>_b.Privaterent</t>
+          <t>_Yesalittle</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Yes a little</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>_d.Other</t>
+          <t>_Yesalot</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Yes a lot</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>_d.PrivateRented</t>
+          <t>_Yesbutnoreducedcapacity</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Yes but no reduced capacity</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>_e.Rent–LA</t>
+          <t>_Yeshavechildren</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Yes have children</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>_f.RentHACoop</t>
+          <t>_Yesonahousinglist</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Yes on a housing list</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>_g.Other</t>
+          <t>1999</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>_h.Inparentalfamilyhome</t>
+          <t>2000</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>_Tojoinanexistingfamilyorhouseho</t>
+          <t>2001</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>_Tooccupytheentireproperty</t>
+          <t>2002</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>_Yes–inthenextsixmonths</t>
+          <t>2003</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>_Yes–over6monthstolessthan1year</t>
+          <t>2004</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>_Yes–over1yearlessthan2years</t>
+          <t>2005</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>_Yes–over2yearslessthan3years</t>
+          <t>2006</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>_Yes–over3yearslessthan4years</t>
+          <t>2007</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>_Yes–over4yearslessthan5years</t>
+          <t>2008</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>_Yes–morethan5years</t>
+          <t>2009</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>_No–dontexpecttomove</t>
+          <t>2010</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>_OwnerOccupier</t>
+          <t>2011</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>_LocalAuthorityRent</t>
+          <t>2012</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>_HousingAssociationRent</t>
+          <t>2013</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>_ShelteredSupported</t>
+          <t>2014</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>_Larger</t>
+          <t>2015</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>_Smaller</t>
+          <t>2016</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>_Samesizeascurrent</t>
+          <t>2017</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>_Verygood</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>_Fairlygood</t>
+          <t>age</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Age</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>_Fairlypoor</t>
+          <t>Alladults</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>All adults</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>_Verypoor</t>
+          <t>AnySport</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Any sport</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>_Noopinion</t>
+          <t>AnySportExclWalking</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Any sport excluding walking</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>_Verystrongly</t>
+          <t>base</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Base</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>_Fairlystrongly</t>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Base</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>_Notverystrongly</t>
+          <t>BaseMin</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Base</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>_Notatallstrongly</t>
+          <t>Category</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>_Verysatisfied</t>
+          <t>CLIMATE1</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>_Fairlysatisfied</t>
+          <t>CLIMATE2_A</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Opinion</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>_Neithersatisfiednordissatisfied</t>
+          <t>CLIMATE2_B</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Opinion</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>_Fairlydissatisfied</t>
+          <t>CLIMATE2_C</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Opinion</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>_Verydissatisfied</t>
+          <t>CLIMATE2_D</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Opinion</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>t25_2018</t>
+          <t>council</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Council</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>t38dep</t>
+          <t>Council</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>_landlord</t>
+          <t>CultAny</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Cultural Engagement</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>_Lettingagent</t>
+          <t>description</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>social1</t>
+          <t>Description</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>_Urbanareas</t>
+          <t>dyear</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>_Ruralareas</t>
+          <t>Experience</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>_Refusal</t>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Gender</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>social2</t>
+          <t>greenfar13</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Walking distance</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>_PrivateRented</t>
+          <t>ha5</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Age</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>_SocialRented</t>
+          <t>ha6</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Gender</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>_Owned</t>
+          <t>ha7</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Economic status</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>_Yes_Disc</t>
+          <t>hb1</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Property type</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>_No_Disc</t>
+          <t>hc6</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Internet Access</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>_Yes_Harass</t>
+          <t>hedqual8</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Education</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>_No_Harass</t>
+          <t>hf1an</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Long-term physical or mental health condition</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>_Yes_Discrim</t>
+          <t>hhtype</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Household type</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>_No_Discrim</t>
+          <t>hhtype_new</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Household type</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>Base</t>
+          <t>hihage</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Highest Age</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>RESIL1</t>
+          <t>hk2</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Status</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>_AllSIMD</t>
+          <t>LABEL</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>dyear</t>
+          <t>net1</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>_Stronglyagree</t>
+          <t>NET6C2018</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>_Tendtoagree</t>
+          <t>outdoor</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Frequency</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>_Neitheragreenordisagree</t>
+          <t>pa1</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>_Tendtodisagree</t>
+          <t>Perception</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>_Stronglydisagree</t>
+          <t>previoustenure</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>_Owneroccupied</t>
+          <t>ra1</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>_Socialrented</t>
+          <t>ra15</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Status</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>_Privaterented</t>
+          <t>rand_id</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Sexual orientation</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>_Anotherway</t>
+          <t>randeth</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Ethnicity</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>hedqual8</t>
+          <t>randstat</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Marital status</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>_Identifiedinanotherway</t>
+          <t>rb1</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Rating</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>_All_Gender</t>
+          <t>RESIL1</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Preparation</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>_16to39</t>
+          <t>response</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>_40to59</t>
+          <t>RESPONSE</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>_All_Age</t>
+          <t>rg5a</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Long-term physical or mental health condition</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>_015000</t>
+          <t>rndrel09</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Religious and ethnic belonging</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>_DegreeProfessionalQualification</t>
+          <t>serv1h</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Opinion</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>_HigherAlevelOGradeStandardGrade</t>
+          <t>serv3a</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Satisfaction</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>_Longtermcondition_1</t>
+          <t>shs_6cla</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Urban/rural classification</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>_nolongtermcondition_1</t>
+          <t>SIMDquintiles</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>SIMD Quintiles</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>_All_1</t>
+          <t>social1</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Frequency</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>_Longtermcondition_2</t>
+          <t>social2</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Frequency</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>_nolongtermcondition_2</t>
+          <t>SPRT3B</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Frequency</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>_All_2</t>
+          <t>t25_2018</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>_Mainincomefromearnings</t>
+          <t>t38dep</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>_Mainincomefrombenefits</t>
+          <t>tenure</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Tenure</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>_Mainincomefromothersources</t>
+          <t>tenurealt</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>_Anequalmixofincomesources</t>
+          <t>tothinc</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Total Income</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>_AllGender</t>
+          <t>var</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>_AllAge</t>
+          <t>vol32018</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Frequency</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>_3000140000</t>
+          <t>vol42018</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Hours</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>_Over40000</t>
+          <t>volinform</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Informal volunteering</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>_Ownbuyownhome</t>
+          <t>voliv2</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Frequency</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>_Rentprivatelandlord</t>
+          <t>voliv3</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Hours</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>_Rentsocialhousing</t>
+          <t>voluntee</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Volunteers</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>NET6C2018</t>
+          <t>Walking</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>serv3a</t>
+          <t>working_adults</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Number of working adults</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>Workingageadults</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Working age adults</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>serv1h</t>
+          <t>Year</t>
         </is>
       </c>
     </row>

</xml_diff>